<commit_message>
EMTF_vu13p_r23 update (links map)
</commit_message>
<xml_diff>
--- a/examples/EMTF_vu13p_r23/src/vu13p_r23.xlsx
+++ b/examples/EMTF_vu13p_r23/src/vu13p_r23.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="vu13p_gty_refclk" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
     <t xml:space="preserve">// path</t>
   </si>
   <si>
-    <t xml:space="preserve">boards/vu13p_gty</t>
+    <t xml:space="preserve">boards/vu13p_r23_gty</t>
   </si>
   <si>
     <t xml:space="preserve">// file</t>
@@ -644,8 +644,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E57" activeCellId="0" sqref="E57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1779,8 +1779,8 @@
   </sheetPr>
   <dimension ref="A1:E132"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>